<commit_message>
upgrades menu flavor text and stuff
neat
</commit_message>
<xml_diff>
--- a/UpgradesFlavorText.xlsx
+++ b/UpgradesFlavorText.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\Documents\BraveLittleVacuum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B02CDD-0C9B-4DF2-80CA-3624BF748812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3554C688-1166-4526-921D-4B1765662FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23115" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{C6C83A6A-9F8F-47CC-A4A6-47682BDE5992}"/>
+    <workbookView xWindow="18345" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{C6C83A6A-9F8F-47CC-A4A6-47682BDE5992}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,24 +101,9 @@
     <t>Low-current brushless motors will keep your SuckMate effortlessly navigating your home for efficient cleaning</t>
   </si>
   <si>
-    <t>Select the Nozzle with E or Q
-Objects fired will cause extra damage. Consumes Power.</t>
-  </si>
-  <si>
     <t>Originally designed with its military applications in mind before it was discovered that it was more economical to just build dedicated war robots than to repurpose household assistants.</t>
   </si>
   <si>
-    <t>Provides power to special upgrades.
-1 Power Supply upgrade collected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provides high voltage auxiliary power to modules that may be unable to </t>
-  </si>
-  <si>
-    <t>Select the Nozzle with E or Q
-Must be charged up before firing by holding LMB.  Does a lot of extra damage and consumes power.</t>
-  </si>
-  <si>
     <t>Prevents damage from being submerged in water</t>
   </si>
   <si>
@@ -128,14 +113,6 @@
     <t>Incoming damage is halved</t>
   </si>
   <si>
-    <t>An aftermarket Nozzle attachment with no real practical purpose. It's pretty fun to use though
-WARNING! Objects expelled from the tank may be travelling at unwise speeds</t>
-  </si>
-  <si>
-    <t>Made from an extremely resistant and durable polymer, bumps and scrapes that would normally damage the unit are instead effortlessly repelled.
-Unfortunately, even a small can of it costs as much as most houses.</t>
-  </si>
-  <si>
     <t>Press Space to jump</t>
   </si>
   <si>
@@ -145,14 +122,31 @@
     <t>Press Space when in the air to hover for a short time</t>
   </si>
   <si>
-    <t>During the skateboard shortage of '99, this popular black market mod allowed many hooligans to still shred using the most unlikely of vehicles.  Many fatalaties happened as a result.</t>
-  </si>
-  <si>
-    <t>Keep places that were once unreachable clean, saves a bundle by not having to buy an entirely SuckMate per floor of your hose.
-Not that many peole can afford houses with more than one floor these days</t>
-  </si>
-  <si>
     <t>Placeholder hover nozzle flavor text</t>
+  </si>
+  <si>
+    <t>Select the Nozzle with E or Q\nObjects fired will cause extra damage. Consumes Power.</t>
+  </si>
+  <si>
+    <t>An aftermarket Nozzle attachment with no real practical use, but very fun.\nWARNING! Objects expelled from the tank may be travelling at unwise speeds</t>
+  </si>
+  <si>
+    <t>Select the Nozzle with E or Q\nMust be charged up before firing by holding LMB.  Does a lot of extra damage and consumes power.</t>
+  </si>
+  <si>
+    <t>Provides power to special upgrades.\n1 Power Supply upgrade collected</t>
+  </si>
+  <si>
+    <t>Provides high voltage auxiliary power to modules that may be unable to run off the Suckmate stock Perpetual Power Supply</t>
+  </si>
+  <si>
+    <t>Made from an extremely resistant and durable polymer, bumps and scrapes that would normally damage the unit are instead effortlessly repelled.\nUnfortunately, even a small can of it costs as much as most houses.</t>
+  </si>
+  <si>
+    <t>Keep places that were once unreachable clean, saves a bundle by not having to buy an entirely SuckMate per floor of your hose.\nNot that many peole can afford houses with more than one floor these days</t>
+  </si>
+  <si>
+    <t>During the skateboard shortage of '99, this popular black market mod allowed many hooligans to still shred using the most unlikely of vehicles.  Many fatalaties were reported.</t>
   </si>
 </sst>
 </file>
@@ -191,10 +185,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06D41EA-3F2A-4AD5-9D53-EBD24DE69274}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +515,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,91 +528,91 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>30</v>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -627,44 +621,44 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>